<commit_message>
Version 1.0 avec Documentation
</commit_message>
<xml_diff>
--- a/Doc/Journal de bord.xlsx
+++ b/Doc/Journal de bord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timothee\CLionProjects\Bataille-navale\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A3B10B-C831-4412-9340-8F340CE073D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F572AA07-6827-4B8B-ABEF-F9C38B033E65}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5CD79DA9-5221-4172-963D-ED5E747AE188}"/>
+    <workbookView xWindow="19068" yWindow="3612" windowWidth="7500" windowHeight="9348" xr2:uid="{5CD79DA9-5221-4172-963D-ED5E747AE188}"/>
   </bookViews>
   <sheets>
     <sheet name="journal" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -102,12 +102,6 @@
     <t>Création des scénarios</t>
   </si>
   <si>
-    <t>Git + Github</t>
-  </si>
-  <si>
-    <t>Instalation git + création dépôt github</t>
-  </si>
-  <si>
     <t>Maquette</t>
   </si>
   <si>
@@ -168,13 +162,31 @@
     <t>Création 3ème map</t>
   </si>
   <si>
-    <t>Selection de maps aléatoire</t>
-  </si>
-  <si>
     <t>Effacer</t>
   </si>
   <si>
-    <t>Efface l'écran au fure et a mesure</t>
+    <t>Version 1.0</t>
+  </si>
+  <si>
+    <t>Rendu de la Version 1.0</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Rendu de la Documentation</t>
+  </si>
+  <si>
+    <t>Git + GitHub</t>
+  </si>
+  <si>
+    <t>Installation git + création dépôt GitHub</t>
+  </si>
+  <si>
+    <t>Sélection de maps aléatoire</t>
+  </si>
+  <si>
+    <t>Efface l'écran au fur et à mesure</t>
   </si>
 </sst>
 </file>
@@ -605,11 +617,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE54EA1-5D7B-45ED-AEBE-57CEB38716ED}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,10 +777,10 @@
         <v>13</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="J5" s="9"/>
     </row>
@@ -794,10 +806,10 @@
         <v>13</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J6" s="9"/>
     </row>
@@ -823,10 +835,10 @@
         <v>14</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J7" s="9"/>
     </row>
@@ -852,10 +864,10 @@
         <v>14</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -881,10 +893,10 @@
         <v>14</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J9" s="9"/>
     </row>
@@ -910,10 +922,10 @@
         <v>14</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J10" s="9"/>
     </row>
@@ -939,10 +951,10 @@
         <v>14</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J11" s="9"/>
     </row>
@@ -961,17 +973,17 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6">
-        <f>IF(AND(C12&lt;&gt;"",D12&lt;&gt;""),D12-C12-E12,"")</f>
+        <f t="shared" ref="F12:F21" si="2">IF(AND(C12&lt;&gt;"",D12&lt;&gt;""),D12-C12-E12,"")</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J12" s="9"/>
     </row>
@@ -990,17 +1002,17 @@
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6">
-        <f>IF(AND(C13&lt;&gt;"",D13&lt;&gt;""),D13-C13-E13,"")</f>
+        <f t="shared" si="2"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J13" s="9"/>
     </row>
@@ -1019,17 +1031,17 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6">
-        <f>IF(AND(C14&lt;&gt;"",D14&lt;&gt;""),D14-C14-E14,"")</f>
+        <f t="shared" si="2"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J14" s="9"/>
     </row>
@@ -1048,17 +1060,17 @@
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6">
-        <f>IF(AND(C15&lt;&gt;"",D15&lt;&gt;""),D15-C15-E15,"")</f>
+        <f t="shared" si="2"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J15" s="9"/>
     </row>
@@ -1077,17 +1089,17 @@
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6">
-        <f>IF(AND(C16&lt;&gt;"",D16&lt;&gt;""),D16-C16-E16,"")</f>
+        <f t="shared" si="2"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J16" s="9"/>
     </row>
@@ -1106,17 +1118,17 @@
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6">
-        <f>IF(AND(C17&lt;&gt;"",D17&lt;&gt;""),D17-C17-E17,"")</f>
+        <f t="shared" si="2"/>
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="J17" s="9"/>
     </row>
@@ -1135,17 +1147,17 @@
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6">
-        <f>IF(AND(C18&lt;&gt;"",D18&lt;&gt;""),D18-C18-E18,"")</f>
+        <f t="shared" si="2"/>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J18" s="9"/>
     </row>
@@ -1164,19 +1176,69 @@
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6">
-        <f>IF(AND(C19&lt;&gt;"",D19&lt;&gt;""),D19-C19-E19,"")</f>
+        <f t="shared" si="2"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>43929</v>
+      </c>
+      <c r="B20" s="11">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>43929</v>
+      </c>
+      <c r="B21" s="11">
+        <v>7</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="9"/>
+      <c r="J21" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1188,7 +1250,7 @@
           <x14:formula1>
             <xm:f>listes!$2:$2</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G19</xm:sqref>
+          <xm:sqref>G2:G21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1265,6 +1327,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FEB7924ED8B1A24180D5ACE015F77795" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4568a5a6c2fa997ab6ebb40e0105d4f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="04c9fcc8-6688-426c-a709-ab5d9d154b1b" xmlns:ns4="a1b92501-ed98-452d-b672-e3645125226c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ddf32da8d8ce642d47dc65b5fde44d1" ns3:_="" ns4:_="">
     <xsd:import namespace="04c9fcc8-6688-426c-a709-ab5d9d154b1b"/>
@@ -1467,15 +1538,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1483,6 +1545,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FBA01F4-C232-4C39-99F0-6B4F3770E020}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2001114-AC85-4781-A30A-BEE39CA014C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1497,14 +1567,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FBA01F4-C232-4C39-99F0-6B4F3770E020}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>